<commit_message>
add major revision data
</commit_message>
<xml_diff>
--- a/results/data/F1_score_recall.xlsx
+++ b/results/data/F1_score_recall.xlsx
@@ -5,13 +5,30 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 2" sheetId="1" r:id="rId4"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet 1" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+  <si>
+    <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
+  </si>
+  <si>
+    <t>Numbers Sheet Name</t>
+  </si>
+  <si>
+    <t>Numbers Table Name</t>
+  </si>
+  <si>
+    <t>Excel Worksheet Name</t>
+  </si>
+  <si>
+    <t>Sheet 2</t>
+  </si>
   <si>
     <t>Table 1</t>
   </si>
@@ -64,10 +81,16 @@
     <t>openmeetings</t>
   </si>
   <si>
+    <t>Deepseek-coder</t>
+  </si>
+  <si>
     <t>Starcoder</t>
   </si>
   <si>
     <t>RefGen</t>
+  </si>
+  <si>
+    <t>Sheet 1</t>
   </si>
 </sst>
 </file>
@@ -77,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -86,6 +109,17 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -110,7 +144,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,18 +159,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -146,14 +198,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -161,68 +213,158 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="19"/>
+      </left>
+      <right style="thin">
+        <color indexed="20"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="19"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="20"/>
+      </left>
+      <right style="thin">
+        <color indexed="19"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="19"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="19"/>
+      </left>
+      <right style="thin">
+        <color indexed="19"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="19"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="19"/>
+      </left>
+      <right style="thin">
+        <color indexed="20"/>
+      </right>
+      <top style="thin">
+        <color indexed="19"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="19"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="20"/>
+      </left>
+      <right style="thin">
+        <color indexed="19"/>
+      </right>
+      <top style="thin">
+        <color indexed="19"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="19"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="19"/>
+      </left>
+      <right style="thin">
+        <color indexed="19"/>
+      </right>
+      <top style="thin">
+        <color indexed="19"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="19"/>
       </bottom>
       <diagonal/>
     </border>
@@ -232,41 +374,95 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -286,12 +482,18 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1323,688 +1525,1315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="4" width="33.6016" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="50" customHeight="1">
+      <c r="B3" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D10" location="'Sheet 2'!R1C1" tooltip="" display="Sheet 2"/>
+    <hyperlink ref="D12" location="'Sheet 1'!R2C1" tooltip="" display="Sheet 1"/>
+  </hyperlinks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="A1" t="s" s="7">
+        <v>5</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" ht="14.35" customHeight="1">
-      <c r="A2" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="5">
+      <c r="A2" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="14.7" customHeight="1">
+      <c r="A3" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.774</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.78</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.777</v>
+      </c>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.785</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.803</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.793</v>
+      </c>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.771</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.8090000000000001</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.765</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.799</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.782</v>
+      </c>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.806</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.823</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.8149999999999999</v>
+      </c>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.785</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.819</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.802</v>
+      </c>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.765</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0.787</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0.776</v>
+      </c>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="17">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0.788</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.801</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.795</v>
+      </c>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.764</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.78</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.787</v>
+      </c>
+    </row>
+    <row r="12" ht="14.7" customHeight="1">
+      <c r="A12" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0.795</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.803</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.801</v>
+      </c>
+    </row>
+    <row r="13" ht="14.7" customHeight="1">
+      <c r="A13" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.781</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.8110000000000001</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.801</v>
+      </c>
+    </row>
+    <row r="14" ht="14.7" customHeight="1">
+      <c r="A14" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0.775</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.8090000000000001</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.802</v>
+      </c>
+    </row>
+    <row r="15" ht="14.7" customHeight="1">
+      <c r="A15" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.806</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.833</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.825</v>
+      </c>
+    </row>
+    <row r="16" ht="14.7" customHeight="1">
+      <c r="A16" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0.795</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.819</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.8120000000000001</v>
+      </c>
+    </row>
+    <row r="17" ht="14.7" customHeight="1">
+      <c r="A17" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0.795</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0.787</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0.796</v>
+      </c>
+    </row>
+    <row r="18" ht="14.7" customHeight="1">
+      <c r="A18" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0.8080000000000001</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.821</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0.821</v>
+      </c>
+    </row>
+    <row r="19" ht="14.7" customHeight="1">
+      <c r="A19" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D19" s="14">
+        <v>0.739</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.715</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0.727</v>
+      </c>
+    </row>
+    <row r="20" ht="14.7" customHeight="1">
+      <c r="A20" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.705</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.722</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0.714</v>
+      </c>
+    </row>
+    <row r="21" ht="14.7" customHeight="1">
+      <c r="A21" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.736</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0.781</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="22" ht="14.7" customHeight="1">
+      <c r="A22" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0.696</v>
+      </c>
+      <c r="E22" s="14">
+        <v>0.731</v>
+      </c>
+      <c r="F22" s="14">
+        <v>0.714</v>
+      </c>
+    </row>
+    <row r="23" ht="14.7" customHeight="1">
+      <c r="A23" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0.722</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0.759</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="24" ht="14.7" customHeight="1">
+      <c r="A24" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D24" s="14">
+        <v>0.711</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0.731</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0.721</v>
+      </c>
+    </row>
+    <row r="25" ht="14.7" customHeight="1">
+      <c r="A25" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D25" s="14">
+        <v>0.736</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0.751</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0.744</v>
+      </c>
+    </row>
+    <row r="26" ht="14.7" customHeight="1">
+      <c r="A26" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="D26" s="14">
+        <v>0.735</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0.73</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.733</v>
+      </c>
+    </row>
+    <row r="27" ht="14.7" customHeight="1">
+      <c r="A27" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D27" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="E27" s="14">
+        <v>0.704</v>
+      </c>
+      <c r="F27" s="14">
+        <v>0.726</v>
+      </c>
+    </row>
+    <row r="28" ht="14.7" customHeight="1">
+      <c r="A28" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0.737</v>
+      </c>
+      <c r="E28" s="14">
+        <v>0.724</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="29" ht="14.7" customHeight="1">
+      <c r="A29" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D29" s="14">
+        <v>0.753</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0.704</v>
+      </c>
+      <c r="F29" s="14">
+        <v>0.728</v>
+      </c>
+    </row>
+    <row r="30" ht="14.7" customHeight="1">
+      <c r="A30" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D30" s="14">
+        <v>0.77</v>
+      </c>
+      <c r="E30" s="14">
+        <v>0.704</v>
+      </c>
+      <c r="F30" s="14">
+        <v>0.736</v>
+      </c>
+    </row>
+    <row r="31" ht="14.7" customHeight="1">
+      <c r="A31" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D31" s="14">
+        <v>0.735</v>
+      </c>
+      <c r="E31" s="14">
+        <v>0.718</v>
+      </c>
+      <c r="F31" s="14">
+        <v>0.726</v>
+      </c>
+    </row>
+    <row r="32" ht="14.7" customHeight="1">
+      <c r="A32" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D32" s="14">
+        <v>0.735</v>
+      </c>
+      <c r="E32" s="14">
+        <v>0.68</v>
+      </c>
+      <c r="F32" s="14">
+        <v>0.707</v>
+      </c>
+    </row>
+    <row r="33" ht="14.7" customHeight="1">
+      <c r="A33" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D33" s="14">
+        <v>0.772</v>
+      </c>
+      <c r="E33" s="14">
+        <v>0.68</v>
+      </c>
+      <c r="F33" s="14">
+        <v>0.723</v>
+      </c>
+    </row>
+    <row r="34" ht="14.7" customHeight="1">
+      <c r="A34" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D34" s="14">
+        <v>0.755</v>
+      </c>
+      <c r="E34" s="14">
+        <v>0.702</v>
+      </c>
+      <c r="F34" s="14">
+        <v>0.728</v>
+      </c>
+    </row>
+    <row r="35" ht="14.7" customHeight="1">
+      <c r="A35" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D35" s="14">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="E35" s="14">
+        <v>0.678</v>
+      </c>
+      <c r="F35" s="14">
+        <v>0.6840000000000001</v>
+      </c>
+    </row>
+    <row r="36" ht="14.7" customHeight="1">
+      <c r="A36" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D36" s="14">
+        <v>0.716</v>
+      </c>
+      <c r="E36" s="14">
+        <v>0.6909999999999999</v>
+      </c>
+      <c r="F36" s="14">
+        <v>0.704</v>
+      </c>
+    </row>
+    <row r="37" ht="14.7" customHeight="1">
+      <c r="A37" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D37" s="14">
+        <v>0.6919999999999999</v>
+      </c>
+      <c r="E37" s="14">
+        <v>0.666</v>
+      </c>
+      <c r="F37" s="14">
+        <v>0.679</v>
+      </c>
+    </row>
+    <row r="38" ht="14.7" customHeight="1">
+      <c r="A38" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D38" s="14">
+        <v>0.6820000000000001</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0.697</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.6889999999999999</v>
+      </c>
+    </row>
+    <row r="39" ht="14.7" customHeight="1">
+      <c r="A39" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D39" s="14">
+        <v>0.739</v>
+      </c>
+      <c r="E39" s="14">
+        <v>0.677</v>
+      </c>
+      <c r="F39" s="14">
+        <v>0.707</v>
+      </c>
+    </row>
+    <row r="40" ht="14.7" customHeight="1">
+      <c r="A40" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D40" s="14">
+        <v>0.705</v>
+      </c>
+      <c r="E40" s="14">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="F40" s="14">
+        <v>0.694</v>
+      </c>
+    </row>
+    <row r="41" ht="14.7" customHeight="1">
+      <c r="A41" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D41" s="14">
+        <v>0.711</v>
+      </c>
+      <c r="E41" s="14">
+        <v>0.677</v>
+      </c>
+      <c r="F41" s="14">
+        <v>0.694</v>
+      </c>
+    </row>
+    <row r="42" ht="14.7" customHeight="1">
+      <c r="A42" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s" s="17">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D42" s="14">
+        <v>0.6820000000000001</v>
+      </c>
+      <c r="E42" s="14">
+        <v>0.72</v>
+      </c>
+      <c r="F42" s="14">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="43" ht="14.7" customHeight="1">
+      <c r="A43" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="C43" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D43" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="E43" s="14">
+        <v>0.704</v>
+      </c>
+      <c r="F43" s="14">
+        <v>0.726</v>
+      </c>
+    </row>
+    <row r="44" ht="14.7" customHeight="1">
+      <c r="A44" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C44" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D44" s="14">
+        <v>0.737</v>
+      </c>
+      <c r="E44" s="14">
+        <v>0.724</v>
+      </c>
+      <c r="F44" s="14">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="45" ht="14.7" customHeight="1">
+      <c r="A45" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D45" s="14">
+        <v>0.753</v>
+      </c>
+      <c r="E45" s="14">
+        <v>0.704</v>
+      </c>
+      <c r="F45" s="14">
+        <v>0.728</v>
+      </c>
+    </row>
+    <row r="46" ht="14.7" customHeight="1">
+      <c r="A46" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C46" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D46" s="14">
+        <v>0.77</v>
+      </c>
+      <c r="E46" s="14">
+        <v>0.704</v>
+      </c>
+      <c r="F46" s="14">
+        <v>0.736</v>
+      </c>
+    </row>
+    <row r="47" ht="14.7" customHeight="1">
+      <c r="A47" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D47" s="14">
+        <v>0.735</v>
+      </c>
+      <c r="E47" s="14">
+        <v>0.718</v>
+      </c>
+      <c r="F47" s="14">
+        <v>0.726</v>
+      </c>
+    </row>
+    <row r="48" ht="14.7" customHeight="1">
+      <c r="A48" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="B48" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D48" s="14">
+        <v>0.735</v>
+      </c>
+      <c r="E48" s="14">
+        <v>0.68</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0.707</v>
+      </c>
+    </row>
+    <row r="49" ht="14.7" customHeight="1">
+      <c r="A49" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D49" s="14">
+        <v>0.772</v>
+      </c>
+      <c r="E49" s="14">
+        <v>0.68</v>
+      </c>
+      <c r="F49" s="14">
+        <v>0.723</v>
+      </c>
+    </row>
+    <row r="50" ht="14.7" customHeight="1">
+      <c r="A50" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s" s="15">
+        <v>22</v>
+      </c>
+      <c r="C50" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="D50" s="14">
+        <v>0.755</v>
+      </c>
+      <c r="E50" s="14">
+        <v>0.702</v>
+      </c>
+      <c r="F50" s="14">
+        <v>0.728</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B4" xSplit="1" ySplit="3" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="6" width="16.3516" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" customHeight="1">
+      <c r="A1" t="s" s="20">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="5">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" ht="14.7" customHeight="1">
+      <c r="A2" t="s" s="10">
         <v>6</v>
       </c>
+      <c r="B2" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="10">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" ht="14.7" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.774</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="A3" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s" s="21">
+        <v>14</v>
+      </c>
+      <c r="D3" s="22">
+        <v>0.764</v>
+      </c>
+      <c r="E3" s="22">
         <v>0.78</v>
       </c>
-      <c r="F3" s="9">
-        <v>0.777</v>
+      <c r="F3" s="22">
+        <v>0.787</v>
       </c>
     </row>
     <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.785</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="A4" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="23">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.795</v>
+      </c>
+      <c r="E4" s="22">
         <v>0.803</v>
       </c>
-      <c r="F4" s="9">
-        <v>0.793</v>
+      <c r="F4" s="22">
+        <v>0.801</v>
       </c>
     </row>
     <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.771</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="A5" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s" s="23">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.781</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.8110000000000001</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0.801</v>
+      </c>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s" s="23">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.775</v>
+      </c>
+      <c r="E6" s="22">
         <v>0.8090000000000001</v>
       </c>
-      <c r="F5" s="9">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.765</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0.799</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0.782</v>
+      <c r="F6" s="22">
+        <v>0.802</v>
       </c>
     </row>
     <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="A7" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s" s="23">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="D7" s="22">
         <v>0.806</v>
       </c>
-      <c r="E7" s="9">
-        <v>0.823</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0.8149999999999999</v>
+      <c r="E7" s="22">
+        <v>0.833</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.825</v>
       </c>
     </row>
     <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.785</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="A8" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s" s="23">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.795</v>
+      </c>
+      <c r="E8" s="22">
         <v>0.819</v>
       </c>
-      <c r="F8" s="9">
-        <v>0.802</v>
+      <c r="F8" s="22">
+        <v>0.8120000000000001</v>
       </c>
     </row>
     <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.765</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="A9" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="23">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="D9" s="22">
+        <v>0.795</v>
+      </c>
+      <c r="E9" s="22">
         <v>0.787</v>
       </c>
-      <c r="F9" s="9">
-        <v>0.776</v>
+      <c r="F9" s="22">
+        <v>0.796</v>
       </c>
     </row>
     <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.788</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.801</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0.795</v>
-      </c>
-    </row>
-    <row r="11" ht="14.7" customHeight="1">
-      <c r="A11" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0.739</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.715</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.727</v>
-      </c>
-    </row>
-    <row r="12" ht="14.7" customHeight="1">
-      <c r="A12" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0.705</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0.722</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0.714</v>
-      </c>
-    </row>
-    <row r="13" ht="14.7" customHeight="1">
-      <c r="A13" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.736</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.781</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0.758</v>
-      </c>
-    </row>
-    <row r="14" ht="14.7" customHeight="1">
-      <c r="A14" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.696</v>
-      </c>
-      <c r="E14" s="9">
-        <v>0.731</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0.714</v>
-      </c>
-    </row>
-    <row r="15" ht="14.7" customHeight="1">
-      <c r="A15" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0.722</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0.759</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="16" ht="14.7" customHeight="1">
-      <c r="A16" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0.711</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0.731</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0.721</v>
-      </c>
-    </row>
-    <row r="17" ht="14.7" customHeight="1">
-      <c r="A17" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0.736</v>
-      </c>
-      <c r="E17" s="9">
-        <v>0.751</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0.744</v>
-      </c>
-    </row>
-    <row r="18" ht="14.7" customHeight="1">
-      <c r="A18" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0.735</v>
-      </c>
-      <c r="E18" s="9">
-        <v>0.73</v>
-      </c>
-      <c r="F18" s="9">
-        <v>0.733</v>
-      </c>
-    </row>
-    <row r="19" ht="14.7" customHeight="1">
-      <c r="A19" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0.75</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0.704</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0.726</v>
-      </c>
-    </row>
-    <row r="20" ht="14.7" customHeight="1">
-      <c r="A20" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0.737</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0.724</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="21" ht="14.7" customHeight="1">
-      <c r="A21" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.753</v>
-      </c>
-      <c r="E21" s="9">
-        <v>0.704</v>
-      </c>
-      <c r="F21" s="9">
-        <v>0.728</v>
-      </c>
-    </row>
-    <row r="22" ht="14.7" customHeight="1">
-      <c r="A22" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D22" s="9">
-        <v>0.77</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0.704</v>
-      </c>
-      <c r="F22" s="9">
-        <v>0.736</v>
-      </c>
-    </row>
-    <row r="23" ht="14.7" customHeight="1">
-      <c r="A23" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0.735</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0.718</v>
-      </c>
-      <c r="F23" s="9">
-        <v>0.726</v>
-      </c>
-    </row>
-    <row r="24" ht="14.7" customHeight="1">
-      <c r="A24" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0.735</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0.68</v>
-      </c>
-      <c r="F24" s="9">
-        <v>0.707</v>
-      </c>
-    </row>
-    <row r="25" ht="14.7" customHeight="1">
-      <c r="A25" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0.772</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0.68</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0.723</v>
-      </c>
-    </row>
-    <row r="26" ht="14.7" customHeight="1">
-      <c r="A26" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B26" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="C26" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D26" s="9">
-        <v>0.755</v>
-      </c>
-      <c r="E26" s="9">
-        <v>0.702</v>
-      </c>
-      <c r="F26" s="9">
-        <v>0.728</v>
-      </c>
-    </row>
-    <row r="27" ht="14.7" customHeight="1">
-      <c r="A27" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C27" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="E27" s="9">
-        <v>0.678</v>
-      </c>
-      <c r="F27" s="9">
-        <v>0.6840000000000001</v>
-      </c>
-    </row>
-    <row r="28" ht="14.7" customHeight="1">
-      <c r="A28" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D28" s="9">
-        <v>0.716</v>
-      </c>
-      <c r="E28" s="9">
-        <v>0.6909999999999999</v>
-      </c>
-      <c r="F28" s="9">
-        <v>0.704</v>
-      </c>
-    </row>
-    <row r="29" ht="14.7" customHeight="1">
-      <c r="A29" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="B29" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C29" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D29" s="9">
-        <v>0.6919999999999999</v>
-      </c>
-      <c r="E29" s="9">
-        <v>0.666</v>
-      </c>
-      <c r="F29" s="9">
-        <v>0.679</v>
-      </c>
-    </row>
-    <row r="30" ht="14.7" customHeight="1">
-      <c r="A30" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D30" s="9">
-        <v>0.6820000000000001</v>
-      </c>
-      <c r="E30" s="9">
-        <v>0.697</v>
-      </c>
-      <c r="F30" s="9">
-        <v>0.6889999999999999</v>
-      </c>
-    </row>
-    <row r="31" ht="14.7" customHeight="1">
-      <c r="A31" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D31" s="9">
-        <v>0.739</v>
-      </c>
-      <c r="E31" s="9">
-        <v>0.677</v>
-      </c>
-      <c r="F31" s="9">
-        <v>0.707</v>
-      </c>
-    </row>
-    <row r="32" ht="14.7" customHeight="1">
-      <c r="A32" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0.705</v>
-      </c>
-      <c r="E32" s="9">
-        <v>0.6830000000000001</v>
-      </c>
-      <c r="F32" s="9">
-        <v>0.694</v>
-      </c>
-    </row>
-    <row r="33" ht="14.7" customHeight="1">
-      <c r="A33" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="B33" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D33" s="9">
-        <v>0.711</v>
-      </c>
-      <c r="E33" s="9">
-        <v>0.677</v>
-      </c>
-      <c r="F33" s="9">
-        <v>0.694</v>
-      </c>
-    </row>
-    <row r="34" ht="14.7" customHeight="1">
-      <c r="A34" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B34" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C34" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D34" s="9">
-        <v>0.6820000000000001</v>
-      </c>
-      <c r="E34" s="9">
-        <v>0.72</v>
-      </c>
-      <c r="F34" s="9">
-        <v>0.7</v>
-      </c>
+      <c r="A10" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="23">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0.8080000000000001</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.821</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0.821</v>
+      </c>
+    </row>
+    <row r="11" ht="14.35" customHeight="1">
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" ht="14.05" customHeight="1">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>